<commit_message>
Analysis including with dpr compounds.
</commit_message>
<xml_diff>
--- a/West_Side_Aphid_Wf_Data2022.forR.xlsx
+++ b/West_Side_Aphid_Wf_Data2022.forR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bachhami\Box Sync\UCDavis_Buddhi\spraydroplet_analysis\droplet_size_2\westside_aphid_wf2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AEEC28-E698-44D8-ADA7-F749FCABB2EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9877BF-078B-4AFF-8347-A1C4CDC4A1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28200" windowHeight="11745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>